<commit_message>
form now will be created folder for every class
</commit_message>
<xml_diff>
--- a/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
+++ b/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\Excel Class 4-Basic Terminologies and use of Sheets and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45A3375-06D6-42B9-B23C-94F3B7A9ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C6C260-E83E-4128-A6D8-BAC933729983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data  for Class 4" sheetId="1" r:id="rId1"/>
     <sheet name="Class-4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>MS Excel</t>
   </si>
@@ -1445,459 +1445,207 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42EE74D-51DB-4AC7-8753-D3842ECE5E8D}">
-  <dimension ref="B1:M26"/>
+  <dimension ref="B2:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="4.75" customWidth="1"/>
-    <col min="6" max="6" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:13">
-      <c r="B2" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="20" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+    </row>
+    <row r="5" spans="2:3" ht="15">
+      <c r="B5" s="30">
         <v>1</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="C5" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15">
+      <c r="B6" s="30">
         <v>2</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="C6" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15">
+      <c r="B7" s="30">
         <v>3</v>
       </c>
-      <c r="L2" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-    </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="7"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="8"/>
-      <c r="F4" s="25">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="C7" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15">
+      <c r="B8" s="30">
         <v>4</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="24"/>
-    </row>
-    <row r="5" spans="2:13" ht="15">
-      <c r="B5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="25">
-        <v>2</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="C8" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15">
+      <c r="B9" s="30">
         <v>5</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="24"/>
-      <c r="L5" s="30">
-        <v>1</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="15">
-      <c r="B6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="12"/>
-      <c r="F6" s="25">
-        <v>3</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="C9" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15">
+      <c r="B10" s="30">
         <v>6</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="24"/>
-      <c r="L6" s="30">
-        <v>2</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="15">
-      <c r="B7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="25">
-        <v>4</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="C10" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15">
+      <c r="B11" s="30">
         <v>7</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="24"/>
-      <c r="L7" s="30">
-        <v>3</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="15">
-      <c r="B8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="F8" s="25">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="C11" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15">
+      <c r="B12" s="30">
         <v>8</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="24"/>
-      <c r="L8" s="30">
-        <v>4</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="15">
-      <c r="B9" s="14"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="10"/>
-      <c r="F9" s="25">
-        <v>6</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="C12" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15">
+      <c r="B13" s="30">
         <v>9</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="24"/>
-      <c r="L9" s="30">
-        <v>5</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="15">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="F10" s="25">
-        <v>7</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="C13" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15">
+      <c r="B14" s="30">
         <v>10</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="24"/>
-      <c r="L10" s="30">
-        <v>6</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="15">
-      <c r="F11" s="25">
-        <v>8</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="C14" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15">
+      <c r="B15" s="30">
         <v>11</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="24"/>
-      <c r="L11" s="30">
-        <v>7</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="15">
-      <c r="F12" s="25">
-        <v>9</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="C15" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15">
+      <c r="B16" s="30">
         <v>12</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="24"/>
-      <c r="L12" s="30">
-        <v>8</v>
-      </c>
-      <c r="M12" s="31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" ht="15">
-      <c r="F13" s="25">
-        <v>10</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="C16" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15">
+      <c r="B17" s="30">
         <v>13</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="24"/>
-      <c r="L13" s="30">
-        <v>9</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="15">
-      <c r="F14" s="25">
-        <v>11</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="C17" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15">
+      <c r="B18" s="30">
         <v>14</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="24"/>
-      <c r="L14" s="30">
-        <v>10</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="15">
-      <c r="F15" s="25">
-        <v>12</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="C18" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15">
+      <c r="B19" s="30">
         <v>15</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="24"/>
-      <c r="L15" s="30">
-        <v>11</v>
-      </c>
-      <c r="M15" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="15">
-      <c r="F16" s="25">
-        <v>13</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="C19" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15">
+      <c r="B20" s="30">
         <v>16</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="24"/>
-      <c r="L16" s="30">
-        <v>12</v>
-      </c>
-      <c r="M16" s="31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="6:13" ht="15">
-      <c r="F17" s="25">
-        <v>14</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="C20" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15">
+      <c r="B21" s="30">
         <v>17</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="24"/>
-      <c r="L17" s="30">
-        <v>13</v>
-      </c>
-      <c r="M17" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="6:13" ht="15">
-      <c r="F18" s="25">
-        <v>15</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="C21" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15">
+      <c r="B22" s="30">
         <v>18</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="24"/>
-      <c r="L18" s="30">
-        <v>14</v>
-      </c>
-      <c r="M18" s="31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="6:13" ht="15">
-      <c r="F19" s="25">
-        <v>16</v>
-      </c>
-      <c r="G19" s="6" t="s">
+      <c r="C22" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15">
+      <c r="B23" s="30">
         <v>19</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="24"/>
-      <c r="L19" s="30">
-        <v>15</v>
-      </c>
-      <c r="M19" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="6:13" ht="15">
-      <c r="F20" s="25">
-        <v>17</v>
-      </c>
-      <c r="G20" s="6" t="s">
+      <c r="C23" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15">
+      <c r="B24" s="30">
         <v>20</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="24"/>
-      <c r="L20" s="30">
-        <v>16</v>
-      </c>
-      <c r="M20" s="31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="6:13" ht="15">
-      <c r="F21" s="25">
-        <v>18</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="C24" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15">
+      <c r="B25" s="30">
         <v>21</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="24"/>
-      <c r="L21" s="30">
-        <v>17</v>
-      </c>
-      <c r="M21" s="31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="6:13" ht="15">
-      <c r="F22" s="25">
-        <v>19</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="C25" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15">
+      <c r="B26" s="30">
         <v>22</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="24"/>
-      <c r="L22" s="30">
-        <v>18</v>
-      </c>
-      <c r="M22" s="31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="6:13" ht="15">
-      <c r="F23" s="26">
-        <v>20</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="29"/>
-      <c r="L23" s="30">
-        <v>19</v>
-      </c>
-      <c r="M23" s="31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="6:13" ht="15">
-      <c r="L24" s="30">
-        <v>20</v>
-      </c>
-      <c r="M24" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="6:13" ht="15">
-      <c r="L25" s="30">
-        <v>21</v>
-      </c>
-      <c r="M25" s="31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="6:13" ht="15">
-      <c r="L26" s="30">
-        <v>22</v>
-      </c>
-      <c r="M26" s="31" t="s">
+      <c r="C26" s="31" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="L2:M3"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calss 4.1 Data added
</commit_message>
<xml_diff>
--- a/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
+++ b/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\Excel Class 4-Basic Terminologies and use of Sheets and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC233A42-2AD7-409D-90B9-1A8B8C57BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F340A5-E665-4D48-A1AC-604F19699831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="500-rows-data" sheetId="3" r:id="rId2"/>
-    <sheet name="Class-4" sheetId="2" r:id="rId3"/>
+    <sheet name="Class-4-1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="96">
   <si>
     <t>MS Excel</t>
   </si>
@@ -313,12 +313,24 @@
   <si>
     <t>Croissant</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Loss/ Profit</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +387,19 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -732,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -786,9 +811,13 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -816,13 +845,11 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1186,11 +1213,11 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:13">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
         <v>0</v>
@@ -1204,23 +1231,23 @@
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="42"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
       <c r="J3" s="24"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="7"/>
@@ -1644,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2E7844-4503-4FFE-98B6-18614AEAF353}">
   <dimension ref="A1:I501"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1659,22 +1686,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="33" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1797,7 +1824,7 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="34">
         <v>3</v>
       </c>
     </row>
@@ -1820,7 +1847,7 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="35">
         <v>2</v>
       </c>
     </row>
@@ -1863,8 +1890,8 @@
       <c r="F10">
         <v>4.25</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -1885,7 +1912,7 @@
       <c r="F11">
         <v>7</v>
       </c>
-      <c r="H11" s="48"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9">
@@ -1907,7 +1934,7 @@
       <c r="F12">
         <v>2.5499999999999998</v>
       </c>
-      <c r="H12" s="48"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9">
@@ -1929,7 +1956,7 @@
       <c r="F13">
         <v>7</v>
       </c>
-      <c r="H13" s="48"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9">
@@ -1951,7 +1978,7 @@
       <c r="F14">
         <v>3</v>
       </c>
-      <c r="H14" s="48"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9">
@@ -1973,7 +2000,7 @@
       <c r="F15">
         <v>3.1</v>
       </c>
-      <c r="H15" s="49"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9">
@@ -11703,212 +11730,376 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42EE74D-51DB-4AC7-8753-D3842ECE5E8D}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="42"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="2:4" ht="15">
+      <c r="C2" s="48"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+    </row>
+    <row r="4" spans="1:8" ht="18">
+      <c r="E4" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
       <c r="B5" s="30">
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="15">
+      <c r="E5" s="53">
+        <v>43831</v>
+      </c>
+      <c r="F5">
+        <v>4709</v>
+      </c>
+      <c r="G5">
+        <v>1019</v>
+      </c>
+      <c r="H5">
+        <f>F5-G5</f>
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
       <c r="B6" s="30">
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="15">
+      <c r="E6" s="53">
+        <v>43832</v>
+      </c>
+      <c r="F6">
+        <v>4004</v>
+      </c>
+      <c r="G6">
+        <v>1261</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H19" si="0">F6-G6</f>
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
       <c r="B7" s="30">
         <v>3</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15">
+      <c r="E7" s="53">
+        <v>43833</v>
+      </c>
+      <c r="F7">
+        <v>7652</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
       <c r="B8" s="30">
         <v>4</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="15">
+      <c r="E8" s="53">
+        <v>43834</v>
+      </c>
+      <c r="F8">
+        <v>7163</v>
+      </c>
+      <c r="G8">
+        <v>1053</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>6110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
       <c r="B9" s="30">
         <v>5</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="15">
+      <c r="E9" s="53">
+        <v>43835</v>
+      </c>
+      <c r="F9">
+        <v>8362</v>
+      </c>
+      <c r="G9">
+        <v>1417</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>6945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
       <c r="B10" s="30">
         <v>6</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="15">
+      <c r="E10" s="53">
+        <v>43836</v>
+      </c>
+      <c r="F10">
+        <v>8709</v>
+      </c>
+      <c r="G10">
+        <v>1134</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>7575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15">
       <c r="B11" s="30">
         <v>7</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="15">
+      <c r="E11" s="53">
+        <v>43837</v>
+      </c>
+      <c r="F11">
+        <v>4223</v>
+      </c>
+      <c r="G11">
+        <v>1281</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15">
       <c r="B12" s="30">
         <v>8</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="15">
+      <c r="E12" s="53">
+        <v>43838</v>
+      </c>
+      <c r="F12">
+        <v>4856</v>
+      </c>
+      <c r="G12">
+        <v>799</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15">
       <c r="B13" s="30">
         <v>9</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="15">
+      <c r="E13" s="53">
+        <v>43839</v>
+      </c>
+      <c r="F13">
+        <v>1758</v>
+      </c>
+      <c r="G13">
+        <v>601</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15">
       <c r="B14" s="30">
         <v>10</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="15">
-      <c r="B15" s="30">
+      <c r="E14" s="53">
+        <v>43840</v>
+      </c>
+      <c r="F14">
+        <v>4086</v>
+      </c>
+      <c r="G14">
+        <v>696</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="E15" s="53">
+        <v>43841</v>
+      </c>
+      <c r="F15">
+        <v>6777</v>
+      </c>
+      <c r="G15">
+        <v>948</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>5829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="B16" s="30">
         <v>11</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C16" s="32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="15">
-      <c r="B16" s="30">
-        <v>12</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15">
+      <c r="E16" s="53">
+        <v>43842</v>
+      </c>
+      <c r="F16">
+        <v>7175</v>
+      </c>
+      <c r="G16">
+        <v>649</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>6526</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15">
       <c r="B17" s="30">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15">
+        <v>43</v>
+      </c>
+      <c r="E17" s="53">
+        <v>43843</v>
+      </c>
+      <c r="F17">
+        <v>6844</v>
+      </c>
+      <c r="G17">
+        <v>1481</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>5363</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15">
       <c r="B18" s="30">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15">
+        <v>42</v>
+      </c>
+      <c r="E18" s="53">
+        <v>43844</v>
+      </c>
+      <c r="F18">
+        <v>2950</v>
+      </c>
+      <c r="G18">
+        <v>783</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15">
       <c r="B19" s="30">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15">
+        <v>47</v>
+      </c>
+      <c r="E19" s="53">
+        <v>43845</v>
+      </c>
+      <c r="F19">
+        <v>9526</v>
+      </c>
+      <c r="G19">
+        <v>1271</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>8255</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15">
       <c r="B20" s="30">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15">
-      <c r="B21" s="30">
-        <v>17</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15">
-      <c r="B22" s="30">
-        <v>18</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15">
-      <c r="B23" s="30">
-        <v>19</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15">
-      <c r="B24" s="30">
-        <v>20</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15">
-      <c r="B25" s="30">
-        <v>21</v>
-      </c>
-      <c r="C25" s="32" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15">
-      <c r="B26" s="30">
-        <v>22</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C3"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Data for all classes is added in main branch
</commit_message>
<xml_diff>
--- a/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
+++ b/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\Excel Class 4-Basic Terminologies and use of Sheets and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F340A5-E665-4D48-A1AC-604F19699831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC233A42-2AD7-409D-90B9-1A8B8C57BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="500-rows-data" sheetId="3" r:id="rId2"/>
-    <sheet name="Class-4-1" sheetId="2" r:id="rId3"/>
+    <sheet name="Class-4" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="92">
   <si>
     <t>MS Excel</t>
   </si>
@@ -313,24 +313,12 @@
   <si>
     <t>Croissant</t>
   </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Loss/ Profit</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Expenses</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,19 +375,6 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -757,7 +732,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -811,13 +786,9 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,11 +816,13 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1213,11 +1186,11 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:13">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
         <v>0</v>
@@ -1231,23 +1204,23 @@
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="48"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
       <c r="J3" s="24"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="7"/>
@@ -1671,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2E7844-4503-4FFE-98B6-18614AEAF353}">
   <dimension ref="A1:I501"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1686,22 +1659,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="43" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1824,7 +1797,7 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="44">
         <v>3</v>
       </c>
     </row>
@@ -1847,7 +1820,7 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="45">
         <v>2</v>
       </c>
     </row>
@@ -1890,8 +1863,8 @@
       <c r="F10">
         <v>4.25</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -1912,7 +1885,7 @@
       <c r="F11">
         <v>7</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="48"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9">
@@ -1934,7 +1907,7 @@
       <c r="F12">
         <v>2.5499999999999998</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="48"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9">
@@ -1956,7 +1929,7 @@
       <c r="F13">
         <v>7</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="48"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9">
@@ -1978,7 +1951,7 @@
       <c r="F14">
         <v>3</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="48"/>
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9">
@@ -2000,7 +1973,7 @@
       <c r="F15">
         <v>3.1</v>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9">
@@ -11730,376 +11703,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42EE74D-51DB-4AC7-8753-D3842ECE5E8D}">
-  <dimension ref="A2:H20"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="48"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-    </row>
-    <row r="4" spans="1:8" ht="18">
-      <c r="E4" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" s="52" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+      <c r="C2" s="42"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="2:4" ht="15">
       <c r="B5" s="30">
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="53">
-        <v>43831</v>
-      </c>
-      <c r="F5">
-        <v>4709</v>
-      </c>
-      <c r="G5">
-        <v>1019</v>
-      </c>
-      <c r="H5">
-        <f>F5-G5</f>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15">
+    </row>
+    <row r="6" spans="2:4" ht="15">
       <c r="B6" s="30">
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="53">
-        <v>43832</v>
-      </c>
-      <c r="F6">
-        <v>4004</v>
-      </c>
-      <c r="G6">
-        <v>1261</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H19" si="0">F6-G6</f>
-        <v>2743</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
+    </row>
+    <row r="7" spans="2:4" ht="15">
       <c r="B7" s="30">
         <v>3</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="53">
-        <v>43833</v>
-      </c>
-      <c r="F7">
-        <v>7652</v>
-      </c>
-      <c r="G7">
-        <v>3000</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>4652</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+    </row>
+    <row r="8" spans="2:4" ht="15">
       <c r="B8" s="30">
         <v>4</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="53">
-        <v>43834</v>
-      </c>
-      <c r="F8">
-        <v>7163</v>
-      </c>
-      <c r="G8">
-        <v>1053</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>6110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15">
+    </row>
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="30">
         <v>5</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="53">
-        <v>43835</v>
-      </c>
-      <c r="F9">
-        <v>8362</v>
-      </c>
-      <c r="G9">
-        <v>1417</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>6945</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15">
+    </row>
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="30">
         <v>6</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="53">
-        <v>43836</v>
-      </c>
-      <c r="F10">
-        <v>8709</v>
-      </c>
-      <c r="G10">
-        <v>1134</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>7575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15">
+    </row>
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="30">
         <v>7</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="53">
-        <v>43837</v>
-      </c>
-      <c r="F11">
-        <v>4223</v>
-      </c>
-      <c r="G11">
-        <v>1281</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>2942</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15">
+    </row>
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="30">
         <v>8</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="53">
-        <v>43838</v>
-      </c>
-      <c r="F12">
-        <v>4856</v>
-      </c>
-      <c r="G12">
-        <v>799</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>4057</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15">
+    </row>
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="30">
         <v>9</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="53">
-        <v>43839</v>
-      </c>
-      <c r="F13">
-        <v>1758</v>
-      </c>
-      <c r="G13">
-        <v>601</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15">
+    </row>
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="30">
         <v>10</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="53">
-        <v>43840</v>
-      </c>
-      <c r="F14">
-        <v>4086</v>
-      </c>
-      <c r="G14">
-        <v>696</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="E15" s="53">
-        <v>43841</v>
-      </c>
-      <c r="F15">
-        <v>6777</v>
-      </c>
-      <c r="G15">
-        <v>948</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>5829</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15">
+    </row>
+    <row r="15" spans="2:4" ht="15">
+      <c r="B15" s="30">
+        <v>11</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="30">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="53">
-        <v>43842</v>
-      </c>
-      <c r="F16">
-        <v>7175</v>
-      </c>
-      <c r="G16">
-        <v>649</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>6526</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15">
       <c r="B17" s="30">
+        <v>13</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15">
+      <c r="B18" s="30">
+        <v>14</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15">
+      <c r="B19" s="30">
+        <v>15</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15">
+      <c r="B20" s="30">
+        <v>16</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15">
+      <c r="B21" s="30">
+        <v>17</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15">
+      <c r="B22" s="30">
         <v>18</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C22" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15">
+      <c r="B23" s="30">
+        <v>19</v>
+      </c>
+      <c r="C23" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="53">
-        <v>43843</v>
-      </c>
-      <c r="F17">
-        <v>6844</v>
-      </c>
-      <c r="G17">
-        <v>1481</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>5363</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="30">
-        <v>19</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="53">
-        <v>43844</v>
-      </c>
-      <c r="F18">
-        <v>2950</v>
-      </c>
-      <c r="G18">
-        <v>783</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>2167</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="15">
-      <c r="B19" s="30">
+    </row>
+    <row r="24" spans="2:3" ht="15">
+      <c r="B24" s="30">
+        <v>20</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15">
+      <c r="B25" s="30">
         <v>21</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C25" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15">
+      <c r="B26" s="30">
+        <v>22</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="53">
-        <v>43845</v>
-      </c>
-      <c r="F19">
-        <v>9526</v>
-      </c>
-      <c r="G19">
-        <v>1271</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>8255</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15">
-      <c r="B20" s="30">
-        <v>22</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C3"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
class 4.1 data is ready for github
</commit_message>
<xml_diff>
--- a/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
+++ b/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\Excel Class 4-Basic Terminologies and use of Sheets and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC233A42-2AD7-409D-90B9-1A8B8C57BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AED6FED-946F-4D3E-9378-5964E65F9EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="96">
   <si>
     <t>MS Excel</t>
   </si>
@@ -313,12 +313,24 @@
   <si>
     <t>Croissant</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Loss/ Profit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +389,20 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -459,7 +485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -726,13 +752,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -789,6 +852,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -816,13 +886,18 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1186,11 +1261,11 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:13">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
         <v>0</v>
@@ -1204,23 +1279,23 @@
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="42"/>
+      <c r="M2" s="49"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
       <c r="J3" s="24"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="7"/>
@@ -1659,22 +1734,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="34" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1797,7 +1872,7 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="35">
         <v>3</v>
       </c>
     </row>
@@ -1820,7 +1895,7 @@
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="36">
         <v>2</v>
       </c>
     </row>
@@ -1863,8 +1938,8 @@
       <c r="F10">
         <v>4.25</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -1885,7 +1960,7 @@
       <c r="F11">
         <v>7</v>
       </c>
-      <c r="H11" s="48"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9">
@@ -1907,7 +1982,7 @@
       <c r="F12">
         <v>2.5499999999999998</v>
       </c>
-      <c r="H12" s="48"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9">
@@ -1929,7 +2004,7 @@
       <c r="F13">
         <v>7</v>
       </c>
-      <c r="H13" s="48"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9">
@@ -1951,7 +2026,7 @@
       <c r="F14">
         <v>3</v>
       </c>
-      <c r="H14" s="48"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9">
@@ -1973,7 +2048,7 @@
       <c r="F15">
         <v>3.1</v>
       </c>
-      <c r="H15" s="49"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9">
@@ -11703,10 +11778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42EE74D-51DB-4AC7-8753-D3842ECE5E8D}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11714,196 +11789,444 @@
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="42"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="C2" s="49"/>
+    </row>
+    <row r="3" spans="1:8" ht="18">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="E3" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="2:4" ht="15">
+      <c r="E4" s="50">
+        <v>43831</v>
+      </c>
+      <c r="F4">
+        <v>2602</v>
+      </c>
+      <c r="G4">
+        <v>1441</v>
+      </c>
+      <c r="H4">
+        <f>F4-G5</f>
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
       <c r="B5" s="30">
         <v>1</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="15">
+      <c r="E5" s="50">
+        <v>43832</v>
+      </c>
+      <c r="F5">
+        <v>2408</v>
+      </c>
+      <c r="G5">
+        <v>798</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H23" si="0">F5-G6</f>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
       <c r="B6" s="30">
         <v>2</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="15">
+      <c r="E6" s="50">
+        <v>43833</v>
+      </c>
+      <c r="F6">
+        <v>3117</v>
+      </c>
+      <c r="G6">
+        <v>1786</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
       <c r="B7" s="30">
         <v>3</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15">
+      <c r="E7" s="50">
+        <v>43834</v>
+      </c>
+      <c r="F7">
+        <v>3558</v>
+      </c>
+      <c r="G7">
+        <v>773</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
       <c r="B8" s="30">
         <v>4</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="15">
+      <c r="E8" s="50">
+        <v>43835</v>
+      </c>
+      <c r="F8">
+        <v>3583</v>
+      </c>
+      <c r="G8">
+        <v>1473</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
       <c r="B9" s="30">
         <v>5</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="15">
+      <c r="E9" s="50">
+        <v>43836</v>
+      </c>
+      <c r="F9">
+        <v>2962</v>
+      </c>
+      <c r="G9">
+        <v>1781</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
       <c r="B10" s="30">
         <v>6</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="15">
+      <c r="E10" s="50">
+        <v>43837</v>
+      </c>
+      <c r="F10">
+        <v>1339</v>
+      </c>
+      <c r="G10">
+        <v>1019</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>-168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15">
       <c r="B11" s="30">
         <v>7</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="15">
+      <c r="E11" s="50">
+        <v>43838</v>
+      </c>
+      <c r="F11">
+        <v>2388</v>
+      </c>
+      <c r="G11">
+        <v>1507</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15">
       <c r="B12" s="30">
         <v>8</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="15">
+      <c r="E12" s="50">
+        <v>43839</v>
+      </c>
+      <c r="F12">
+        <v>2407</v>
+      </c>
+      <c r="G12">
+        <v>557</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15">
       <c r="B13" s="30">
         <v>9</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="15">
+      <c r="E13" s="50">
+        <v>43840</v>
+      </c>
+      <c r="F13">
+        <v>1865</v>
+      </c>
+      <c r="G13">
+        <v>1038</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15">
       <c r="B14" s="30">
         <v>10</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="15">
+      <c r="E14" s="50">
+        <v>43841</v>
+      </c>
+      <c r="F14">
+        <v>2543</v>
+      </c>
+      <c r="G14">
+        <v>1562</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
       <c r="B15" s="30">
         <v>11</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="15">
-      <c r="B16" s="30">
-        <v>12</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15">
+      <c r="E15" s="50">
+        <v>43842</v>
+      </c>
+      <c r="F15">
+        <v>2931</v>
+      </c>
+      <c r="G15">
+        <v>1532</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="E16" s="50">
+        <v>43843</v>
+      </c>
+      <c r="F16">
+        <v>3074</v>
+      </c>
+      <c r="G16">
+        <v>1247</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15">
       <c r="B17" s="30">
         <v>13</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15">
+        <v>43</v>
+      </c>
+      <c r="E17" s="50">
+        <v>43844</v>
+      </c>
+      <c r="F17">
+        <v>1318</v>
+      </c>
+      <c r="G17">
+        <v>1787</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15">
       <c r="B18" s="30">
         <v>14</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15">
+        <v>42</v>
+      </c>
+      <c r="E18" s="50">
+        <v>43845</v>
+      </c>
+      <c r="F18">
+        <v>1344</v>
+      </c>
+      <c r="G18">
+        <v>864</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>-265</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15">
       <c r="B19" s="30">
         <v>15</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15">
+        <v>47</v>
+      </c>
+      <c r="E19" s="50">
+        <v>43846</v>
+      </c>
+      <c r="F19">
+        <v>3398</v>
+      </c>
+      <c r="G19">
+        <v>1609</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15">
       <c r="B20" s="30">
         <v>16</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15">
+        <v>46</v>
+      </c>
+      <c r="E20" s="50">
+        <v>43847</v>
+      </c>
+      <c r="F20">
+        <v>2651</v>
+      </c>
+      <c r="G20">
+        <v>1712</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" s="30">
         <v>17</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15">
-      <c r="B22" s="30">
-        <v>18</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15">
-      <c r="B23" s="30">
-        <v>19</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15">
-      <c r="B24" s="30">
-        <v>20</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15">
-      <c r="B25" s="30">
-        <v>21</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15">
-      <c r="B26" s="30">
-        <v>22</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>47</v>
-      </c>
+      <c r="E21" s="50">
+        <v>43848</v>
+      </c>
+      <c r="F21">
+        <v>3955</v>
+      </c>
+      <c r="G21">
+        <v>1177</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="30"/>
+      <c r="E22" s="50">
+        <v>43849</v>
+      </c>
+      <c r="F22">
+        <v>3284</v>
+      </c>
+      <c r="G22">
+        <v>1338</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="30"/>
+      <c r="E23" s="50">
+        <v>43850</v>
+      </c>
+      <c r="F23">
+        <v>3599</v>
+      </c>
+      <c r="G23">
+        <v>1429</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>3599</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="30"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="30"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Class 4 data created for excel sheet
</commit_message>
<xml_diff>
--- a/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
+++ b/Excel Class 4-Basic Terminologies and use of Sheets and Data/Excel Class 4-Basic Terminologies and use of Sheets and Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\Excel-YT-Classes-Data\Excel-Classes-Excel-Files\Excel Class 4-Basic Terminologies and use of Sheets and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AED6FED-946F-4D3E-9378-5964E65F9EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE855CC-D4B0-458B-816A-93C5D7AF5729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
@@ -406,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +482,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -859,6 +865,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -886,18 +901,9 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1261,11 +1267,11 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:13">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
         <v>0</v>
@@ -1279,23 +1285,23 @@
       <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="49"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
       <c r="J3" s="24"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="7"/>
@@ -11781,7 +11787,7 @@
   <dimension ref="A2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11790,36 +11796,36 @@
     <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="54"/>
     </row>
     <row r="3" spans="1:8" ht="18">
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="E3" s="51" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="E3" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="57" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="33"/>
-      <c r="E4" s="50">
+      <c r="E4" s="41">
         <v>43831</v>
       </c>
       <c r="F4">
@@ -11840,7 +11846,7 @@
       <c r="C5" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="41">
         <v>43832</v>
       </c>
       <c r="F5">
@@ -11861,7 +11867,7 @@
       <c r="C6" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="41">
         <v>43833</v>
       </c>
       <c r="F6">
@@ -11882,7 +11888,7 @@
       <c r="C7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="41">
         <v>43834</v>
       </c>
       <c r="F7">
@@ -11903,7 +11909,7 @@
       <c r="C8" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="41">
         <v>43835</v>
       </c>
       <c r="F8">
@@ -11924,7 +11930,7 @@
       <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="41">
         <v>43836</v>
       </c>
       <c r="F9">
@@ -11945,7 +11951,7 @@
       <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="41">
         <v>43837</v>
       </c>
       <c r="F10">
@@ -11966,7 +11972,7 @@
       <c r="C11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="41">
         <v>43838</v>
       </c>
       <c r="F11">
@@ -11987,7 +11993,7 @@
       <c r="C12" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="50">
+      <c r="E12" s="41">
         <v>43839</v>
       </c>
       <c r="F12">
@@ -12008,7 +12014,7 @@
       <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="41">
         <v>43840</v>
       </c>
       <c r="F13">
@@ -12029,7 +12035,7 @@
       <c r="C14" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="41">
         <v>43841</v>
       </c>
       <c r="F14">
@@ -12050,7 +12056,7 @@
       <c r="C15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="41">
         <v>43842</v>
       </c>
       <c r="F15">
@@ -12065,10 +12071,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="E16" s="50">
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="E16" s="41">
         <v>43843</v>
       </c>
       <c r="F16">
@@ -12089,7 +12095,7 @@
       <c r="C17" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="41">
         <v>43844</v>
       </c>
       <c r="F17">
@@ -12110,7 +12116,7 @@
       <c r="C18" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="41">
         <v>43845</v>
       </c>
       <c r="F18">
@@ -12131,7 +12137,7 @@
       <c r="C19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="50">
+      <c r="E19" s="41">
         <v>43846</v>
       </c>
       <c r="F19">
@@ -12152,7 +12158,7 @@
       <c r="C20" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="41">
         <v>43847</v>
       </c>
       <c r="F20">
@@ -12170,7 +12176,7 @@
       <c r="B21" s="30">
         <v>17</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="41">
         <v>43848</v>
       </c>
       <c r="F21">
@@ -12186,7 +12192,7 @@
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="30"/>
-      <c r="E22" s="50">
+      <c r="E22" s="41">
         <v>43849</v>
       </c>
       <c r="F22">
@@ -12202,7 +12208,7 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="30"/>
-      <c r="E23" s="50">
+      <c r="E23" s="41">
         <v>43850</v>
       </c>
       <c r="F23">

</xml_diff>